<commit_message>
updated excel with conditions for ABORT
</commit_message>
<xml_diff>
--- a/ProcLib/DOC/Outcomes.xlsx
+++ b/ProcLib/DOC/Outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/lab-schall/Tempo/schalllab-rig029/ProcLib/DOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6376856C-0BB7-8248-BC94-AC39674187A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1E401E-57EB-0341-9927-C69E9085A156}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="-19340" windowWidth="28040" windowHeight="17440" xr2:uid="{9853A192-6172-5B46-9DD3-E6910C72440B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>STATE PROC</t>
   </si>
@@ -114,6 +114,50 @@
   <si>
     <t>NOGO TRIAL 
 (before Stop_Signal)</t>
+  </si>
+  <si>
+    <t>TONE_CHK</t>
+  </si>
+  <si>
+    <t>TRL_TARG_HOLD_BRK_PRE_TONE_TIME</t>
+  </si>
+  <si>
+    <t>TargHoldBrkPreTone_</t>
+  </si>
+  <si>
+    <t>TRL_TARG_HOLD_BRK_TONE_TIME</t>
+  </si>
+  <si>
+    <t>TargHoldBrkTone_</t>
+  </si>
+  <si>
+    <t>TRL_TARG_HOLD_BRK_PRE_RWRD_TIME</t>
+  </si>
+  <si>
+    <t>RWRD_CHK</t>
+  </si>
+  <si>
+    <t>TargHoldBrkPreRwrd_</t>
+  </si>
+  <si>
+    <t>Gaze not in TARG_WIN during Tone
+What tone to be given for NOGO Trial, since this is NoGoWrong?</t>
+  </si>
+  <si>
+    <t>TRL_TARG_HOLD_BRK_RWRD_TIME</t>
+  </si>
+  <si>
+    <t>TargHoldBrkRwrd_</t>
+  </si>
+  <si>
+    <t>Reward is already delivered
+Is this OK for NOGO?</t>
+  </si>
+  <si>
+    <t>TRL_TARG_HOLD_BRK_POST_RWRD_TIME</t>
+  </si>
+  <si>
+    <t>TargHoldBrkPostRwrd_</t>
   </si>
 </sst>
 </file>
@@ -157,13 +201,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,16 +529,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2851BBA-6F7F-0848-8CAF-4B3E85974DCE}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E15" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
@@ -524,83 +574,404 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Excel with Amir for NOGO outcomes
</commit_message>
<xml_diff>
--- a/ProcLib/DOC/Outcomes.xlsx
+++ b/ProcLib/DOC/Outcomes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/lab-schall/Tempo/schalllab-rig029/ProcLib/DOC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tempo\rigProcLibs\schalllab-rig029\ProcLib\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1E401E-57EB-0341-9927-C69E9085A156}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A06A53-FAB3-4492-99FF-B86AAFEEB0B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="-19340" windowWidth="28040" windowHeight="17440" xr2:uid="{9853A192-6172-5B46-9DD3-E6910C72440B}"/>
+    <workbookView xWindow="825" yWindow="285" windowWidth="26970" windowHeight="14490" xr2:uid="{9853A192-6172-5B46-9DD3-E6910C72440B}"/>
   </bookViews>
   <sheets>
     <sheet name="STAT_ABORT" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>STATE PROC</t>
   </si>
@@ -64,9 +59,6 @@
   </si>
   <si>
     <t>TRL_FIX_HOLD_BRK_TIME</t>
-  </si>
-  <si>
-    <t>BreakFix_, Abort_</t>
   </si>
   <si>
     <t>TARG_ON</t>
@@ -140,10 +132,6 @@
     <t>TargHoldBrkPreRwrd_</t>
   </si>
   <si>
-    <t>Gaze not in TARG_WIN during Tone
-What tone to be given for NOGO Trial, since this is NoGoWrong?</t>
-  </si>
-  <si>
     <t>TRL_TARG_HOLD_BRK_RWRD_TIME</t>
   </si>
   <si>
@@ -158,6 +146,16 @@
   </si>
   <si>
     <t>TargHoldBrkPostRwrd_</t>
+  </si>
+  <si>
+    <t>BreakFix_</t>
+  </si>
+  <si>
+    <t>Gaze not in TARG_WIN during Tone
+What tone to be given for NOGO Trial, since this is NoGoError?</t>
+  </si>
+  <si>
+    <t>NoGoError_</t>
   </si>
 </sst>
 </file>
@@ -531,23 +529,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2851BBA-6F7F-0848-8CAF-4B3E85974DCE}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="27.625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,16 +562,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -586,12 +584,18 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -601,7 +605,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -610,14 +614,20 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -627,193 +637,237 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H12" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -823,7 +877,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -833,7 +887,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -843,7 +897,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -853,7 +907,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -863,7 +917,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -873,7 +927,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -883,7 +937,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -893,7 +947,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -903,7 +957,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -913,7 +967,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -923,7 +977,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -933,7 +987,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -943,7 +997,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -953,7 +1007,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -963,7 +1017,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -985,7 +1039,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed event code sending for bitsweep
</commit_message>
<xml_diff>
--- a/ProcLib/DOC/Outcomes.xlsx
+++ b/ProcLib/DOC/Outcomes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tempo\rigProcLibs\schalllab-rig029\ProcLib\DOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/lab-schall/Tempo/schalllab-rig029/ProcLib/DOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A06A53-FAB3-4492-99FF-B86AAFEEB0B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1E401E-57EB-0341-9927-C69E9085A156}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="285" windowWidth="26970" windowHeight="14490" xr2:uid="{9853A192-6172-5B46-9DD3-E6910C72440B}"/>
+    <workbookView xWindow="3000" yWindow="-19340" windowWidth="28040" windowHeight="17440" xr2:uid="{9853A192-6172-5B46-9DD3-E6910C72440B}"/>
   </bookViews>
   <sheets>
     <sheet name="STAT_ABORT" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>STATE PROC</t>
   </si>
@@ -59,6 +64,9 @@
   </si>
   <si>
     <t>TRL_FIX_HOLD_BRK_TIME</t>
+  </si>
+  <si>
+    <t>BreakFix_, Abort_</t>
   </si>
   <si>
     <t>TARG_ON</t>
@@ -132,6 +140,10 @@
     <t>TargHoldBrkPreRwrd_</t>
   </si>
   <si>
+    <t>Gaze not in TARG_WIN during Tone
+What tone to be given for NOGO Trial, since this is NoGoWrong?</t>
+  </si>
+  <si>
     <t>TRL_TARG_HOLD_BRK_RWRD_TIME</t>
   </si>
   <si>
@@ -146,16 +158,6 @@
   </si>
   <si>
     <t>TargHoldBrkPostRwrd_</t>
-  </si>
-  <si>
-    <t>BreakFix_</t>
-  </si>
-  <si>
-    <t>Gaze not in TARG_WIN during Tone
-What tone to be given for NOGO Trial, since this is NoGoError?</t>
-  </si>
-  <si>
-    <t>NoGoError_</t>
   </si>
 </sst>
 </file>
@@ -529,23 +531,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2851BBA-6F7F-0848-8CAF-4B3E85974DCE}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="23.375" customWidth="1"/>
-    <col min="4" max="4" width="27.625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,16 +564,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -584,18 +586,12 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -605,7 +601,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -614,20 +610,14 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -637,237 +627,193 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -877,7 +823,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -887,7 +833,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -897,7 +843,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -907,7 +853,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -917,7 +863,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -927,7 +873,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -937,7 +883,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -947,7 +893,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -957,7 +903,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -967,7 +913,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -977,7 +923,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -987,7 +933,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -997,7 +943,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1007,7 +953,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1017,7 +963,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1039,7 +985,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>